<commit_message>
More filter options and other tweaks
</commit_message>
<xml_diff>
--- a/data/philos_manual-adj.xlsx
+++ b/data/philos_manual-adj.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gregor Große-Bölting\Documents\dev\exiled-philosophers\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4133EC12-E0D1-4F7C-80D0-97E49B158D3C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B046FC0A-AD1A-4DDF-891F-6A33BA361D24}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="787">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="790">
   <si>
     <t>name</t>
   </si>
@@ -2381,6 +2381,15 @@
   </si>
   <si>
     <t>34.05222222222222 -118.0</t>
+  </si>
+  <si>
+    <t>missingDeathDate</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>True</t>
   </si>
 </sst>
 </file>
@@ -2764,24 +2773,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H130"/>
+  <dimension ref="A1:I130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C53" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="52.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="55.109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="57.21875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="41" style="3" customWidth="1"/>
-    <col min="8" max="8" width="63" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="55.109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="57.21875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="41" style="3" customWidth="1"/>
+    <col min="9" max="9" width="63" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2791,23 +2801,26 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>787</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2817,23 +2830,26 @@
       <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>732</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>733</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -2843,23 +2859,26 @@
       <c r="C3" s="5" t="s">
         <v>700</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -2869,23 +2888,26 @@
       <c r="C4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -2895,23 +2917,26 @@
       <c r="C5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>36</v>
       </c>
@@ -2921,23 +2946,26 @@
       <c r="C6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>734</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>735</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>42</v>
       </c>
@@ -2947,23 +2975,26 @@
       <c r="C7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>692</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>691</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -2973,23 +3004,26 @@
       <c r="C8" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>52</v>
       </c>
@@ -2999,23 +3033,26 @@
       <c r="C9" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>60</v>
       </c>
@@ -3025,23 +3062,26 @@
       <c r="C10" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>736</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -3051,23 +3091,26 @@
       <c r="C11" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>74</v>
       </c>
@@ -3077,23 +3120,26 @@
       <c r="C12" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>78</v>
       </c>
@@ -3103,23 +3149,26 @@
       <c r="C13" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>694</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>693</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>84</v>
       </c>
@@ -3129,23 +3178,26 @@
       <c r="C14" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>686</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>685</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>738</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>88</v>
       </c>
@@ -3155,23 +3207,26 @@
       <c r="C15" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>739</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>94</v>
       </c>
@@ -3181,23 +3236,26 @@
       <c r="C16" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>100</v>
       </c>
@@ -3207,23 +3265,26 @@
       <c r="C17" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>742</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>107</v>
       </c>
@@ -3233,23 +3294,26 @@
       <c r="C18" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>113</v>
       </c>
@@ -3259,23 +3323,26 @@
       <c r="C19" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>119</v>
       </c>
@@ -3285,23 +3352,26 @@
       <c r="C20" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>741</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>740</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="I20" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>125</v>
       </c>
@@ -3311,23 +3381,26 @@
       <c r="C21" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>687</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>688</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>131</v>
       </c>
@@ -3337,23 +3410,26 @@
       <c r="C22" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>137</v>
       </c>
@@ -3363,23 +3439,26 @@
       <c r="C23" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="I23" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>145</v>
       </c>
@@ -3389,23 +3468,26 @@
       <c r="C24" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="I24" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>149</v>
       </c>
@@ -3415,23 +3497,26 @@
       <c r="C25" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="H25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="I25" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>153</v>
       </c>
@@ -3441,23 +3526,26 @@
       <c r="C26" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>689</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>690</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>157</v>
       </c>
@@ -3467,19 +3555,22 @@
       <c r="C27" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="2" t="s">
+      <c r="H27" s="2"/>
+      <c r="I27" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>163</v>
       </c>
@@ -3489,23 +3580,26 @@
       <c r="C28" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>743</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>744</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>167</v>
       </c>
@@ -3515,23 +3609,26 @@
       <c r="C29" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="H29" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="I29" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>173</v>
       </c>
@@ -3541,23 +3638,26 @@
       <c r="C30" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="H30" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="I30" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>179</v>
       </c>
@@ -3567,23 +3667,26 @@
       <c r="C31" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>687</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>688</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>185</v>
       </c>
@@ -3593,23 +3696,26 @@
       <c r="C32" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>696</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>697</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="H32" s="2" t="s">
         <v>751</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>189</v>
       </c>
@@ -3619,23 +3725,26 @@
       <c r="C33" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="H33" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="I33" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>195</v>
       </c>
@@ -3645,23 +3754,26 @@
       <c r="C34" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="H34" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="I34" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>201</v>
       </c>
@@ -3671,23 +3783,26 @@
       <c r="C35" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="H35" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="I35" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>205</v>
       </c>
@@ -3697,23 +3812,26 @@
       <c r="C36" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>698</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>699</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="H36" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="I36" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>211</v>
       </c>
@@ -3723,23 +3841,26 @@
       <c r="C37" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="F37" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="G37" s="2" t="s">
         <v>754</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="I37" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>217</v>
       </c>
@@ -3749,23 +3870,26 @@
       <c r="C38" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="F38" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="G38" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="H38" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="I38" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>223</v>
       </c>
@@ -3775,23 +3899,26 @@
       <c r="C39" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="G39" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="H39" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="I39" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>227</v>
       </c>
@@ -3801,23 +3928,26 @@
       <c r="C40" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="G40" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="H40" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="I40" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>233</v>
       </c>
@@ -3827,23 +3957,26 @@
       <c r="C41" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="G41" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="H41" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="I41" s="2" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>237</v>
       </c>
@@ -3853,23 +3986,26 @@
       <c r="C42" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="G42" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="H42" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="I42" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>243</v>
       </c>
@@ -3879,23 +4015,26 @@
       <c r="C43" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="G43" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="H43" s="2" t="s">
         <v>745</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="I43" s="2" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>247</v>
       </c>
@@ -3905,19 +4044,22 @@
       <c r="C44" s="5" t="s">
         <v>747</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="F44" s="2"/>
       <c r="G44" s="2"/>
-      <c r="H44" s="2" t="s">
+      <c r="H44" s="2"/>
+      <c r="I44" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>250</v>
       </c>
@@ -3927,23 +4069,26 @@
       <c r="C45" s="5" t="s">
         <v>748</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="F45" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="G45" s="3" t="s">
         <v>749</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="H45" s="2" t="s">
         <v>750</v>
       </c>
-      <c r="H45" s="2" t="s">
+      <c r="I45" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>255</v>
       </c>
@@ -3953,23 +4098,26 @@
       <c r="C46" s="5" t="s">
         <v>701</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="G46" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="H46" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="H46" s="2" t="s">
+      <c r="I46" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>260</v>
       </c>
@@ -3979,19 +4127,22 @@
       <c r="C47" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="F47" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F47" s="2"/>
       <c r="G47" s="2"/>
-      <c r="H47" s="2" t="s">
+      <c r="H47" s="2"/>
+      <c r="I47" s="2" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>264</v>
       </c>
@@ -4001,23 +4152,26 @@
       <c r="C48" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="G48" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="H48" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="I48" s="2" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>270</v>
       </c>
@@ -4027,23 +4181,26 @@
       <c r="C49" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D49" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="G49" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="H49" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="I49" s="2" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>274</v>
       </c>
@@ -4053,23 +4210,26 @@
       <c r="C50" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D50" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="G50" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="H50" s="2" t="s">
         <v>756</v>
       </c>
-      <c r="H50" s="2" t="s">
+      <c r="I50" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>280</v>
       </c>
@@ -4079,23 +4239,26 @@
       <c r="C51" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="F51" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="G51" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="G51" s="2" t="s">
+      <c r="H51" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="H51" s="2" t="s">
+      <c r="I51" s="2" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>288</v>
       </c>
@@ -4105,23 +4268,26 @@
       <c r="C52" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D52" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="F52" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="G52" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="H52" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="H52" s="2" t="s">
+      <c r="I52" s="2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>292</v>
       </c>
@@ -4131,23 +4297,26 @@
       <c r="C53" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D53" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="F53" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="G53" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="G53" s="2" t="s">
+      <c r="H53" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="H53" s="2" t="s">
+      <c r="I53" s="2" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>298</v>
       </c>
@@ -4157,23 +4326,26 @@
       <c r="C54" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E54" s="3" t="s">
         <v>709</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="F54" s="2" t="s">
         <v>710</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="G54" s="2" t="s">
         <v>720</v>
       </c>
-      <c r="G54" s="2" t="s">
+      <c r="H54" s="2" t="s">
         <v>719</v>
       </c>
-      <c r="H54" s="2" t="s">
+      <c r="I54" s="2" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>302</v>
       </c>
@@ -4183,23 +4355,26 @@
       <c r="C55" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D55" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="G55" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="G55" s="2" t="s">
+      <c r="H55" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="H55" s="2" t="s">
+      <c r="I55" s="2" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>310</v>
       </c>
@@ -4209,23 +4384,26 @@
       <c r="C56" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D56" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="F56" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="G56" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G56" s="2" t="s">
+      <c r="H56" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H56" s="2" t="s">
+      <c r="I56" s="2" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>314</v>
       </c>
@@ -4235,23 +4413,26 @@
       <c r="C57" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D57" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="F57" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="G57" s="2" t="s">
         <v>757</v>
       </c>
-      <c r="G57" s="2" t="s">
+      <c r="H57" s="2" t="s">
         <v>758</v>
       </c>
-      <c r="H57" s="2" t="s">
+      <c r="I57" s="2" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>318</v>
       </c>
@@ -4261,23 +4442,26 @@
       <c r="C58" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D58" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="F58" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="G58" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="H58" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="H58" s="2" t="s">
+      <c r="I58" s="2" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>324</v>
       </c>
@@ -4287,23 +4471,26 @@
       <c r="C59" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D59" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="F59" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="G59" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G59" s="2" t="s">
+      <c r="H59" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="I59" s="2" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>330</v>
       </c>
@@ -4313,23 +4500,26 @@
       <c r="C60" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D60" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>711</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="F60" s="2" t="s">
         <v>712</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="G60" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G60" s="2" t="s">
+      <c r="H60" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H60" s="2" t="s">
+      <c r="I60" s="2" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>334</v>
       </c>
@@ -4339,23 +4529,26 @@
       <c r="C61" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="D61" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="F61" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="F61" s="2" t="s">
+      <c r="G61" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="G61" s="2" t="s">
+      <c r="H61" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="H61" s="2" t="s">
+      <c r="I61" s="2" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>342</v>
       </c>
@@ -4365,23 +4558,26 @@
       <c r="C62" s="5" t="s">
         <v>344</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="D62" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E62" s="2" t="s">
         <v>714</v>
       </c>
-      <c r="E62" s="2" t="s">
+      <c r="F62" s="2" t="s">
         <v>713</v>
       </c>
-      <c r="F62" s="2" t="s">
+      <c r="G62" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G62" s="3" t="s">
+      <c r="H62" s="3" t="s">
         <v>695</v>
       </c>
-      <c r="H62" s="2" t="s">
+      <c r="I62" s="2" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>346</v>
       </c>
@@ -4391,23 +4587,26 @@
       <c r="C63" s="5" t="s">
         <v>348</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="D63" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>715</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="F63" s="2" t="s">
         <v>716</v>
       </c>
-      <c r="F63" s="2" t="s">
+      <c r="G63" s="2" t="s">
         <v>757</v>
       </c>
-      <c r="G63" s="2" t="s">
+      <c r="H63" s="2" t="s">
         <v>758</v>
       </c>
-      <c r="H63" s="2" t="s">
+      <c r="I63" s="2" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>350</v>
       </c>
@@ -4417,23 +4616,26 @@
       <c r="C64" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E64" s="3" t="s">
         <v>717</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="F64" s="2" t="s">
         <v>718</v>
       </c>
-      <c r="F64" s="2" t="s">
+      <c r="G64" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="G64" s="2" t="s">
+      <c r="H64" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="H64" s="2" t="s">
+      <c r="I64" s="2" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>356</v>
       </c>
@@ -4443,23 +4645,26 @@
       <c r="C65" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D65" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="F65" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="F65" s="2" t="s">
+      <c r="G65" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="G65" s="2" t="s">
+      <c r="H65" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="H65" s="2" t="s">
+      <c r="I65" s="2" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>362</v>
       </c>
@@ -4469,23 +4674,26 @@
       <c r="C66" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D66" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="F66" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F66" s="3" t="s">
+      <c r="G66" s="3" t="s">
         <v>759</v>
       </c>
-      <c r="G66" s="2" t="s">
+      <c r="H66" s="2" t="s">
         <v>760</v>
       </c>
-      <c r="H66" s="2" t="s">
+      <c r="I66" s="2" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>366</v>
       </c>
@@ -4495,23 +4703,26 @@
       <c r="C67" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D67" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="F67" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="G67" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G67" s="3" t="s">
+      <c r="H67" s="3" t="s">
         <v>695</v>
       </c>
-      <c r="H67" s="2" t="s">
+      <c r="I67" s="2" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>370</v>
       </c>
@@ -4521,42 +4732,48 @@
       <c r="C68" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="D68" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E68" s="2" t="s">
         <v>720</v>
       </c>
-      <c r="E68" s="2" t="s">
+      <c r="F68" s="2" t="s">
         <v>719</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="G68" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="G68" s="2" t="s">
+      <c r="H68" s="2" t="s">
         <v>785</v>
       </c>
-      <c r="H68" s="2" t="s">
+      <c r="I68" s="2" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>375</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="D69" s="5" t="s">
+        <v>789</v>
+      </c>
+      <c r="E69" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="F69" s="2" t="s">
         <v>723</v>
       </c>
-      <c r="F69" s="2"/>
       <c r="G69" s="2"/>
-      <c r="H69" s="2" t="s">
+      <c r="H69" s="2"/>
+      <c r="I69" s="2" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>379</v>
       </c>
@@ -4566,23 +4783,26 @@
       <c r="C70" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D70" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E70" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E70" s="2" t="s">
+      <c r="F70" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="G70" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="G70" s="2" t="s">
+      <c r="H70" s="2" t="s">
         <v>786</v>
       </c>
-      <c r="H70" s="2" t="s">
+      <c r="I70" s="2" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>384</v>
       </c>
@@ -4592,23 +4812,26 @@
       <c r="C71" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D71" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="F71" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="G71" s="2" t="s">
         <v>757</v>
       </c>
-      <c r="G71" s="3" t="s">
+      <c r="H71" s="3" t="s">
         <v>758</v>
       </c>
-      <c r="H71" s="2" t="s">
+      <c r="I71" s="2" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>388</v>
       </c>
@@ -4618,23 +4841,26 @@
       <c r="C72" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D72" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E72" s="2" t="s">
         <v>722</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="F72" s="2" t="s">
         <v>721</v>
       </c>
-      <c r="F72" s="3" t="s">
+      <c r="G72" s="3" t="s">
         <v>754</v>
       </c>
-      <c r="G72" s="3" t="s">
+      <c r="H72" s="3" t="s">
         <v>753</v>
       </c>
-      <c r="H72" s="2" t="s">
+      <c r="I72" s="2" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>392</v>
       </c>
@@ -4644,23 +4870,26 @@
       <c r="C73" s="5" t="s">
         <v>394</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D73" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E73" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="F73" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F73" s="2" t="s">
+      <c r="G73" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="G73" s="2" t="s">
+      <c r="H73" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="H73" s="2" t="s">
+      <c r="I73" s="2" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>398</v>
       </c>
@@ -4670,23 +4899,26 @@
       <c r="C74" s="5" t="s">
         <v>701</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D74" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E74" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="F74" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="G74" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="G74" s="2" t="s">
+      <c r="H74" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="H74" s="2" t="s">
+      <c r="I74" s="2" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>402</v>
       </c>
@@ -4696,23 +4928,26 @@
       <c r="C75" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D75" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="F75" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="G75" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G75" s="2" t="s">
+      <c r="H75" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H75" s="2" t="s">
+      <c r="I75" s="2" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>406</v>
       </c>
@@ -4722,23 +4957,26 @@
       <c r="C76" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D76" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E76" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="F76" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F76" s="2" t="s">
+      <c r="G76" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="G76" s="2" t="s">
+      <c r="H76" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="H76" s="2" t="s">
+      <c r="I76" s="2" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>412</v>
       </c>
@@ -4748,23 +4986,26 @@
       <c r="C77" s="5" t="s">
         <v>414</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D77" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E77" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="F77" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F77" s="3" t="s">
+      <c r="G77" s="3" t="s">
         <v>752</v>
       </c>
-      <c r="G77" s="3" t="s">
+      <c r="H77" s="3" t="s">
         <v>751</v>
       </c>
-      <c r="H77" s="2" t="s">
+      <c r="I77" s="2" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>416</v>
       </c>
@@ -4774,23 +5015,26 @@
       <c r="C78" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="D78" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E78" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="F78" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="G78" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="G78" s="2" t="s">
+      <c r="H78" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="H78" s="2" t="s">
+      <c r="I78" s="2" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>424</v>
       </c>
@@ -4800,23 +5044,26 @@
       <c r="C79" s="5" t="s">
         <v>426</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="D79" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E79" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="F79" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="G79" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G79" s="2" t="s">
+      <c r="H79" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H79" s="2" t="s">
+      <c r="I79" s="2" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>428</v>
       </c>
@@ -4826,23 +5073,26 @@
       <c r="C80" s="5" t="s">
         <v>430</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="D80" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E80" s="2" t="s">
         <v>724</v>
       </c>
-      <c r="E80" s="2" t="s">
+      <c r="F80" s="2" t="s">
         <v>725</v>
       </c>
-      <c r="F80" s="2" t="s">
+      <c r="G80" s="2" t="s">
         <v>761</v>
       </c>
-      <c r="G80" s="2" t="s">
+      <c r="H80" s="2" t="s">
         <v>762</v>
       </c>
-      <c r="H80" s="2" t="s">
+      <c r="I80" s="2" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>432</v>
       </c>
@@ -4852,23 +5102,26 @@
       <c r="C81" s="5" t="s">
         <v>434</v>
       </c>
-      <c r="D81" s="2" t="s">
+      <c r="D81" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E81" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="F81" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="G81" s="2" t="s">
         <v>763</v>
       </c>
-      <c r="G81" s="2" t="s">
+      <c r="H81" s="2" t="s">
         <v>764</v>
       </c>
-      <c r="H81" s="2" t="s">
+      <c r="I81" s="2" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>438</v>
       </c>
@@ -4878,23 +5131,26 @@
       <c r="C82" s="5" t="s">
         <v>440</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="D82" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E82" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="E82" s="2" t="s">
+      <c r="F82" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="F82" s="2" t="s">
+      <c r="G82" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="G82" s="2" t="s">
+      <c r="H82" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="H82" s="2" t="s">
+      <c r="I82" s="2" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>444</v>
       </c>
@@ -4904,42 +5160,48 @@
       <c r="C83" s="5" t="s">
         <v>446</v>
       </c>
-      <c r="D83" s="2" t="s">
+      <c r="D83" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E83" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E83" s="2" t="s">
+      <c r="F83" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F83" s="2" t="s">
+      <c r="G83" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="G83" s="2" t="s">
+      <c r="H83" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="H83" s="2" t="s">
+      <c r="I83" s="2" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>450</v>
       </c>
       <c r="B84" s="5" t="s">
         <v>702</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="D84" s="5" t="s">
+        <v>789</v>
+      </c>
+      <c r="E84" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E84" s="2" t="s">
+      <c r="F84" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F84" s="2"/>
       <c r="G84" s="2"/>
-      <c r="H84" s="2" t="s">
+      <c r="H84" s="2"/>
+      <c r="I84" s="2" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>452</v>
       </c>
@@ -4949,23 +5211,26 @@
       <c r="C85" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="D85" s="3" t="s">
+      <c r="D85" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E85" s="3" t="s">
         <v>726</v>
       </c>
-      <c r="E85" s="2" t="s">
+      <c r="F85" s="2" t="s">
         <v>727</v>
       </c>
-      <c r="F85" s="2" t="s">
+      <c r="G85" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G85" s="2" t="s">
+      <c r="H85" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H85" s="2" t="s">
+      <c r="I85" s="2" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>456</v>
       </c>
@@ -4975,23 +5240,26 @@
       <c r="C86" s="5" t="s">
         <v>458</v>
       </c>
-      <c r="D86" s="2" t="s">
+      <c r="D86" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E86" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="E86" s="2" t="s">
+      <c r="F86" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="F86" s="3" t="s">
+      <c r="G86" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G86" s="2" t="s">
+      <c r="H86" s="2" t="s">
         <v>765</v>
       </c>
-      <c r="H86" s="2" t="s">
+      <c r="I86" s="2" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>462</v>
       </c>
@@ -5001,23 +5269,26 @@
       <c r="C87" s="5" t="s">
         <v>464</v>
       </c>
-      <c r="D87" s="2" t="s">
+      <c r="D87" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E87" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="E87" s="2" t="s">
+      <c r="F87" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="F87" s="2" t="s">
+      <c r="G87" s="2" t="s">
         <v>767</v>
       </c>
-      <c r="G87" s="2" t="s">
+      <c r="H87" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="H87" s="2" t="s">
+      <c r="I87" s="2" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>468</v>
       </c>
@@ -5027,23 +5298,26 @@
       <c r="C88" s="5" t="s">
         <v>470</v>
       </c>
-      <c r="D88" s="2" t="s">
+      <c r="D88" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E88" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E88" s="2" t="s">
+      <c r="F88" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="F88" s="2" t="s">
+      <c r="G88" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G88" s="2" t="s">
+      <c r="H88" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="H88" s="2" t="s">
+      <c r="I88" s="2" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>472</v>
       </c>
@@ -5053,23 +5327,26 @@
       <c r="C89" s="5" t="s">
         <v>474</v>
       </c>
-      <c r="D89" s="2" t="s">
+      <c r="D89" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E89" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E89" s="2" t="s">
+      <c r="F89" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F89" s="2" t="s">
+      <c r="G89" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G89" s="2" t="s">
+      <c r="H89" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H89" s="2" t="s">
+      <c r="I89" s="2" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>476</v>
       </c>
@@ -5079,23 +5356,26 @@
       <c r="C90" s="5" t="s">
         <v>478</v>
       </c>
-      <c r="D90" s="2" t="s">
+      <c r="D90" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E90" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E90" s="2" t="s">
+      <c r="F90" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="F90" s="3" t="s">
+      <c r="G90" s="3" t="s">
         <v>768</v>
       </c>
-      <c r="G90" s="2" t="s">
+      <c r="H90" s="2" t="s">
         <v>769</v>
       </c>
-      <c r="H90" s="2" t="s">
+      <c r="I90" s="2" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>480</v>
       </c>
@@ -5105,23 +5385,26 @@
       <c r="C91" s="5" t="s">
         <v>482</v>
       </c>
-      <c r="D91" s="2" t="s">
+      <c r="D91" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E91" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E91" s="2" t="s">
+      <c r="F91" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F91" s="2" t="s">
+      <c r="G91" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="G91" s="2" t="s">
+      <c r="H91" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="H91" s="2" t="s">
+      <c r="I91" s="2" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>486</v>
       </c>
@@ -5131,23 +5414,26 @@
       <c r="C92" s="5" t="s">
         <v>488</v>
       </c>
-      <c r="D92" s="2" t="s">
+      <c r="D92" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E92" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E92" s="2" t="s">
+      <c r="F92" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F92" s="2" t="s">
+      <c r="G92" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="G92" s="2" t="s">
+      <c r="H92" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="H92" s="2" t="s">
+      <c r="I92" s="2" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>492</v>
       </c>
@@ -5157,23 +5443,26 @@
       <c r="C93" s="5" t="s">
         <v>494</v>
       </c>
-      <c r="D93" s="2" t="s">
+      <c r="D93" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E93" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E93" s="2" t="s">
+      <c r="F93" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F93" s="2" t="s">
+      <c r="G93" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G93" s="2" t="s">
+      <c r="H93" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H93" s="2" t="s">
+      <c r="I93" s="2" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>496</v>
       </c>
@@ -5183,23 +5472,26 @@
       <c r="C94" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="D94" s="2" t="s">
+      <c r="D94" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E94" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="E94" s="2" t="s">
+      <c r="F94" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="F94" s="2" t="s">
+      <c r="G94" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G94" s="2" t="s">
+      <c r="H94" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="H94" s="2" t="s">
+      <c r="I94" s="2" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>500</v>
       </c>
@@ -5209,23 +5501,26 @@
       <c r="C95" s="5" t="s">
         <v>704</v>
       </c>
-      <c r="D95" s="3" t="s">
+      <c r="D95" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E95" s="3" t="s">
         <v>724</v>
       </c>
-      <c r="E95" s="2" t="s">
+      <c r="F95" s="2" t="s">
         <v>725</v>
       </c>
-      <c r="F95" s="3" t="s">
+      <c r="G95" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G95" s="3" t="s">
+      <c r="H95" s="3" t="s">
         <v>695</v>
       </c>
-      <c r="H95" s="2" t="s">
+      <c r="I95" s="2" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>502</v>
       </c>
@@ -5235,23 +5530,26 @@
       <c r="C96" s="5" t="s">
         <v>504</v>
       </c>
-      <c r="D96" s="2" t="s">
+      <c r="D96" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E96" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="E96" s="2" t="s">
+      <c r="F96" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="F96" s="2" t="s">
+      <c r="G96" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="G96" s="2" t="s">
+      <c r="H96" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="H96" s="2" t="s">
+      <c r="I96" s="2" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>508</v>
       </c>
@@ -5261,23 +5559,26 @@
       <c r="C97" s="5" t="s">
         <v>510</v>
       </c>
-      <c r="D97" s="2" t="s">
+      <c r="D97" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E97" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E97" s="2" t="s">
+      <c r="F97" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F97" s="3" t="s">
+      <c r="G97" s="3" t="s">
         <v>770</v>
       </c>
-      <c r="G97" s="2" t="s">
+      <c r="H97" s="2" t="s">
         <v>771</v>
       </c>
-      <c r="H97" s="2" t="s">
+      <c r="I97" s="2" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>512</v>
       </c>
@@ -5287,23 +5588,26 @@
       <c r="C98" s="5" t="s">
         <v>513</v>
       </c>
-      <c r="D98" s="2" t="s">
+      <c r="D98" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E98" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="E98" s="2" t="s">
+      <c r="F98" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="F98" s="2" t="s">
+      <c r="G98" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="G98" s="2" t="s">
+      <c r="H98" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="H98" s="2" t="s">
+      <c r="I98" s="2" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>517</v>
       </c>
@@ -5313,42 +5617,48 @@
       <c r="C99" s="5" t="s">
         <v>519</v>
       </c>
-      <c r="D99" s="2" t="s">
+      <c r="D99" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E99" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E99" s="2" t="s">
+      <c r="F99" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F99" s="2" t="s">
+      <c r="G99" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="G99" s="2" t="s">
+      <c r="H99" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="H99" s="2" t="s">
+      <c r="I99" s="2" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>523</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>706</v>
       </c>
-      <c r="D100" s="2" t="s">
+      <c r="D100" s="5" t="s">
+        <v>789</v>
+      </c>
+      <c r="E100" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E100" s="2" t="s">
+      <c r="F100" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F100" s="2"/>
       <c r="G100" s="2"/>
-      <c r="H100" s="2" t="s">
+      <c r="H100" s="2"/>
+      <c r="I100" s="2" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>525</v>
       </c>
@@ -5358,46 +5668,52 @@
       <c r="C101" s="5" t="s">
         <v>527</v>
       </c>
-      <c r="D101" s="2" t="s">
+      <c r="D101" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E101" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="E101" s="2" t="s">
+      <c r="F101" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="F101" s="2" t="s">
+      <c r="G101" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="G101" s="2" t="s">
+      <c r="H101" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="H101" s="2" t="s">
+      <c r="I101" s="2" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>533</v>
       </c>
       <c r="B102" s="5" t="s">
         <v>707</v>
       </c>
-      <c r="D102" s="2" t="s">
+      <c r="D102" s="5" t="s">
+        <v>789</v>
+      </c>
+      <c r="E102" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="E102" s="2" t="s">
+      <c r="F102" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="F102" s="3" t="s">
+      <c r="G102" s="3" t="s">
         <v>772</v>
       </c>
-      <c r="G102" s="2" t="s">
+      <c r="H102" s="2" t="s">
         <v>773</v>
       </c>
-      <c r="H102" s="2" t="s">
+      <c r="I102" s="2" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>537</v>
       </c>
@@ -5407,23 +5723,26 @@
       <c r="C103" s="5" t="s">
         <v>539</v>
       </c>
-      <c r="D103" s="2" t="s">
+      <c r="D103" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E103" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="E103" s="2" t="s">
+      <c r="F103" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="F103" s="2" t="s">
+      <c r="G103" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G103" s="2" t="s">
+      <c r="H103" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H103" s="2" t="s">
+      <c r="I103" s="2" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>543</v>
       </c>
@@ -5433,23 +5752,26 @@
       <c r="C104" s="5" t="s">
         <v>545</v>
       </c>
-      <c r="D104" s="2" t="s">
+      <c r="D104" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E104" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="E104" s="2" t="s">
+      <c r="F104" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="F104" s="2" t="s">
+      <c r="G104" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="G104" s="2" t="s">
+      <c r="H104" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H104" s="2" t="s">
+      <c r="I104" s="2" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>551</v>
       </c>
@@ -5459,23 +5781,26 @@
       <c r="C105" s="5" t="s">
         <v>553</v>
       </c>
-      <c r="D105" s="2" t="s">
+      <c r="D105" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E105" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="E105" s="2" t="s">
+      <c r="F105" s="2" t="s">
         <v>555</v>
       </c>
-      <c r="F105" s="2" t="s">
+      <c r="G105" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G105" s="2" t="s">
+      <c r="H105" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H105" s="2" t="s">
+      <c r="I105" s="2" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>557</v>
       </c>
@@ -5485,23 +5810,26 @@
       <c r="C106" s="5" t="s">
         <v>559</v>
       </c>
-      <c r="D106" s="2" t="s">
+      <c r="D106" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E106" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E106" s="2" t="s">
+      <c r="F106" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F106" s="2" t="s">
+      <c r="G106" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G106" s="2" t="s">
+      <c r="H106" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H106" s="2" t="s">
+      <c r="I106" s="2" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>561</v>
       </c>
@@ -5511,23 +5839,26 @@
       <c r="C107" s="5" t="s">
         <v>563</v>
       </c>
-      <c r="D107" s="2" t="s">
+      <c r="D107" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E107" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E107" s="2" t="s">
+      <c r="F107" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F107" s="2" t="s">
+      <c r="G107" s="2" t="s">
         <v>774</v>
       </c>
-      <c r="G107" s="2" t="s">
+      <c r="H107" s="2" t="s">
         <v>775</v>
       </c>
-      <c r="H107" s="2" t="s">
+      <c r="I107" s="2" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>565</v>
       </c>
@@ -5537,23 +5868,26 @@
       <c r="C108" s="5" t="s">
         <v>567</v>
       </c>
-      <c r="D108" s="3" t="s">
+      <c r="D108" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E108" s="3" t="s">
         <v>729</v>
       </c>
-      <c r="E108" s="2" t="s">
+      <c r="F108" s="2" t="s">
         <v>730</v>
       </c>
-      <c r="F108" s="2" t="s">
+      <c r="G108" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G108" s="2" t="s">
+      <c r="H108" s="2" t="s">
         <v>742</v>
       </c>
-      <c r="H108" s="2" t="s">
+      <c r="I108" s="2" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>569</v>
       </c>
@@ -5563,23 +5897,26 @@
       <c r="C109" s="5" t="s">
         <v>571</v>
       </c>
-      <c r="D109" s="2" t="s">
+      <c r="D109" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E109" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="E109" s="2" t="s">
+      <c r="F109" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="F109" s="2" t="s">
+      <c r="G109" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G109" s="2" t="s">
+      <c r="H109" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H109" s="2" t="s">
+      <c r="I109" s="2" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>575</v>
       </c>
@@ -5589,19 +5926,22 @@
       <c r="C110" s="5" t="s">
         <v>577</v>
       </c>
-      <c r="D110" s="2" t="s">
+      <c r="D110" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E110" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E110" s="2" t="s">
+      <c r="F110" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F110" s="2"/>
       <c r="G110" s="2"/>
-      <c r="H110" s="2" t="s">
+      <c r="H110" s="2"/>
+      <c r="I110" s="2" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>579</v>
       </c>
@@ -5611,23 +5951,26 @@
       <c r="C111" s="5" t="s">
         <v>581</v>
       </c>
-      <c r="D111" s="2" t="s">
+      <c r="D111" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E111" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E111" s="2" t="s">
+      <c r="F111" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F111" s="2" t="s">
+      <c r="G111" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G111" s="2" t="s">
+      <c r="H111" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="H111" s="2" t="s">
+      <c r="I111" s="2" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>583</v>
       </c>
@@ -5637,23 +5980,26 @@
       <c r="C112" s="5" t="s">
         <v>585</v>
       </c>
-      <c r="D112" s="2" t="s">
+      <c r="D112" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E112" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="E112" s="2" t="s">
+      <c r="F112" s="2" t="s">
         <v>587</v>
       </c>
-      <c r="F112" s="2" t="s">
+      <c r="G112" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G112" s="3" t="s">
+      <c r="H112" s="3" t="s">
         <v>695</v>
       </c>
-      <c r="H112" s="2" t="s">
+      <c r="I112" s="2" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>589</v>
       </c>
@@ -5663,23 +6009,26 @@
       <c r="C113" s="5" t="s">
         <v>591</v>
       </c>
-      <c r="D113" s="2" t="s">
+      <c r="D113" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E113" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="E113" s="2" t="s">
+      <c r="F113" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="F113" s="2" t="s">
+      <c r="G113" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G113" s="2" t="s">
+      <c r="H113" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H113" s="2" t="s">
+      <c r="I113" s="2" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>595</v>
       </c>
@@ -5689,23 +6038,26 @@
       <c r="C114" s="5" t="s">
         <v>597</v>
       </c>
-      <c r="D114" s="2" t="s">
+      <c r="D114" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E114" s="2" t="s">
         <v>598</v>
       </c>
-      <c r="E114" s="2" t="s">
+      <c r="F114" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="F114" s="3" t="s">
+      <c r="G114" s="3" t="s">
         <v>776</v>
       </c>
-      <c r="G114" s="2" t="s">
+      <c r="H114" s="2" t="s">
         <v>777</v>
       </c>
-      <c r="H114" s="2" t="s">
+      <c r="I114" s="2" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>601</v>
       </c>
@@ -5715,23 +6067,26 @@
       <c r="C115" s="5" t="s">
         <v>603</v>
       </c>
-      <c r="D115" s="2" t="s">
+      <c r="D115" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E115" s="2" t="s">
         <v>604</v>
       </c>
-      <c r="E115" s="2" t="s">
+      <c r="F115" s="2" t="s">
         <v>605</v>
       </c>
-      <c r="F115" s="2" t="s">
+      <c r="G115" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G115" s="2" t="s">
+      <c r="H115" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H115" s="2" t="s">
+      <c r="I115" s="2" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>607</v>
       </c>
@@ -5741,23 +6096,26 @@
       <c r="C116" s="5" t="s">
         <v>779</v>
       </c>
-      <c r="D116" s="2" t="s">
+      <c r="D116" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E116" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E116" s="2" t="s">
+      <c r="F116" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F116" s="3" t="s">
+      <c r="G116" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="G116" s="2" t="s">
+      <c r="H116" s="2" t="s">
         <v>778</v>
       </c>
-      <c r="H116" s="2" t="s">
+      <c r="I116" s="2" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>609</v>
       </c>
@@ -5767,23 +6125,26 @@
       <c r="C117" s="5" t="s">
         <v>611</v>
       </c>
-      <c r="D117" s="2" t="s">
+      <c r="D117" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E117" s="2" t="s">
         <v>612</v>
       </c>
-      <c r="E117" s="2" t="s">
+      <c r="F117" s="2" t="s">
         <v>731</v>
       </c>
-      <c r="F117" s="2" t="s">
+      <c r="G117" s="2" t="s">
         <v>613</v>
       </c>
-      <c r="G117" s="2" t="s">
+      <c r="H117" s="2" t="s">
         <v>614</v>
       </c>
-      <c r="H117" s="2" t="s">
+      <c r="I117" s="2" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>616</v>
       </c>
@@ -5793,23 +6154,26 @@
       <c r="C118" s="5" t="s">
         <v>618</v>
       </c>
-      <c r="D118" s="2" t="s">
+      <c r="D118" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E118" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E118" s="2" t="s">
+      <c r="F118" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F118" s="2" t="s">
+      <c r="G118" s="2" t="s">
         <v>619</v>
       </c>
-      <c r="G118" s="2" t="s">
+      <c r="H118" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="H118" s="2" t="s">
+      <c r="I118" s="2" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>622</v>
       </c>
@@ -5819,23 +6183,26 @@
       <c r="C119" s="5" t="s">
         <v>624</v>
       </c>
-      <c r="D119" s="2" t="s">
+      <c r="D119" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E119" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E119" s="2" t="s">
+      <c r="F119" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F119" s="2" t="s">
+      <c r="G119" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G119" s="2" t="s">
+      <c r="H119" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H119" s="2" t="s">
+      <c r="I119" s="2" t="s">
         <v>625</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>626</v>
       </c>
@@ -5845,23 +6212,26 @@
       <c r="C120" s="5" t="s">
         <v>628</v>
       </c>
-      <c r="D120" s="2" t="s">
+      <c r="D120" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E120" s="2" t="s">
         <v>720</v>
       </c>
-      <c r="E120" s="2" t="s">
+      <c r="F120" s="2" t="s">
         <v>719</v>
       </c>
-      <c r="F120" s="2" t="s">
+      <c r="G120" s="2" t="s">
         <v>629</v>
       </c>
-      <c r="G120" s="2" t="s">
+      <c r="H120" s="2" t="s">
         <v>630</v>
       </c>
-      <c r="H120" s="2" t="s">
+      <c r="I120" s="2" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>632</v>
       </c>
@@ -5871,23 +6241,26 @@
       <c r="C121" s="5" t="s">
         <v>634</v>
       </c>
-      <c r="D121" s="2" t="s">
+      <c r="D121" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E121" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E121" s="2" t="s">
+      <c r="F121" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F121" s="2" t="s">
+      <c r="G121" s="2" t="s">
         <v>635</v>
       </c>
-      <c r="G121" s="2" t="s">
+      <c r="H121" s="2" t="s">
         <v>636</v>
       </c>
-      <c r="H121" s="2" t="s">
+      <c r="I121" s="2" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>638</v>
       </c>
@@ -5897,23 +6270,26 @@
       <c r="C122" s="5" t="s">
         <v>640</v>
       </c>
-      <c r="D122" s="2" t="s">
+      <c r="D122" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E122" s="2" t="s">
         <v>641</v>
       </c>
-      <c r="E122" s="2" t="s">
+      <c r="F122" s="2" t="s">
         <v>642</v>
       </c>
-      <c r="F122" s="2" t="s">
+      <c r="G122" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G122" s="2" t="s">
+      <c r="H122" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H122" s="2" t="s">
+      <c r="I122" s="2" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>644</v>
       </c>
@@ -5923,23 +6299,26 @@
       <c r="C123" s="5" t="s">
         <v>646</v>
       </c>
-      <c r="D123" s="2" t="s">
+      <c r="D123" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E123" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E123" s="2" t="s">
+      <c r="F123" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F123" s="3" t="s">
+      <c r="G123" s="3" t="s">
         <v>780</v>
       </c>
-      <c r="G123" s="2" t="s">
+      <c r="H123" s="2" t="s">
         <v>781</v>
       </c>
-      <c r="H123" s="2" t="s">
+      <c r="I123" s="2" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>648</v>
       </c>
@@ -5949,23 +6328,26 @@
       <c r="C124" s="5" t="s">
         <v>650</v>
       </c>
-      <c r="D124" s="2" t="s">
+      <c r="D124" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E124" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E124" s="2" t="s">
+      <c r="F124" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F124" s="2" t="s">
+      <c r="G124" s="2" t="s">
         <v>635</v>
       </c>
-      <c r="G124" s="2" t="s">
+      <c r="H124" s="2" t="s">
         <v>636</v>
       </c>
-      <c r="H124" s="2" t="s">
+      <c r="I124" s="2" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>652</v>
       </c>
@@ -5975,23 +6357,26 @@
       <c r="C125" s="5" t="s">
         <v>654</v>
       </c>
-      <c r="D125" s="2" t="s">
+      <c r="D125" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E125" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="E125" s="2" t="s">
+      <c r="F125" s="2" t="s">
         <v>656</v>
       </c>
-      <c r="F125" s="2" t="s">
+      <c r="G125" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="G125" s="2" t="s">
+      <c r="H125" s="2" t="s">
         <v>656</v>
       </c>
-      <c r="H125" s="2" t="s">
+      <c r="I125" s="2" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>658</v>
       </c>
@@ -6001,23 +6386,26 @@
       <c r="C126" s="5" t="s">
         <v>660</v>
       </c>
-      <c r="D126" s="2" t="s">
+      <c r="D126" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E126" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="E126" s="2" t="s">
+      <c r="F126" s="2" t="s">
         <v>662</v>
       </c>
-      <c r="F126" s="2" t="s">
+      <c r="G126" s="2" t="s">
         <v>663</v>
       </c>
-      <c r="G126" s="2" t="s">
+      <c r="H126" s="2" t="s">
         <v>664</v>
       </c>
-      <c r="H126" s="2" t="s">
+      <c r="I126" s="2" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>666</v>
       </c>
@@ -6027,23 +6415,26 @@
       <c r="C127" s="5" t="s">
         <v>668</v>
       </c>
-      <c r="D127" s="2" t="s">
+      <c r="D127" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E127" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="E127" s="2" t="s">
+      <c r="F127" s="2" t="s">
         <v>662</v>
       </c>
-      <c r="F127" s="2" t="s">
+      <c r="G127" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="G127" s="2" t="s">
+      <c r="H127" s="2" t="s">
         <v>784</v>
       </c>
-      <c r="H127" s="2" t="s">
+      <c r="I127" s="2" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>670</v>
       </c>
@@ -6053,23 +6444,26 @@
       <c r="C128" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="D128" s="2" t="s">
+      <c r="D128" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E128" s="2" t="s">
         <v>673</v>
       </c>
-      <c r="E128" s="2" t="s">
+      <c r="F128" s="2" t="s">
         <v>674</v>
       </c>
-      <c r="F128" s="2" t="s">
+      <c r="G128" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G128" s="2" t="s">
+      <c r="H128" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="H128" s="2" t="s">
+      <c r="I128" s="2" t="s">
         <v>675</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>676</v>
       </c>
@@ -6079,23 +6473,26 @@
       <c r="C129" s="5" t="s">
         <v>678</v>
       </c>
-      <c r="D129" s="2" t="s">
+      <c r="D129" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E129" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E129" s="2" t="s">
+      <c r="F129" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F129" s="2" t="s">
+      <c r="G129" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="G129" s="2" t="s">
+      <c r="H129" s="2" t="s">
         <v>680</v>
       </c>
-      <c r="H129" s="2" t="s">
+      <c r="I129" s="2" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>682</v>
       </c>
@@ -6105,25 +6502,28 @@
       <c r="C130" s="5" t="s">
         <v>701</v>
       </c>
-      <c r="D130" s="2" t="s">
+      <c r="D130" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E130" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E130" s="2" t="s">
+      <c r="F130" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F130" s="2" t="s">
+      <c r="G130" s="2" t="s">
         <v>783</v>
       </c>
-      <c r="G130" s="2" t="s">
+      <c r="H130" s="2" t="s">
         <v>782</v>
       </c>
-      <c r="H130" s="2" t="s">
+      <c r="I130" s="2" t="s">
         <v>684</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{BD47B93E-0347-422F-AF44-2DF152A78624}"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{BD47B93E-0347-422F-AF44-2DF152A78624}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Added coloring by gender and descriptive text
</commit_message>
<xml_diff>
--- a/data/philos_manual-adj.xlsx
+++ b/data/philos_manual-adj.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gregor Große-Bölting\Documents\dev\exiled-philosophers\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B046FC0A-AD1A-4DDF-891F-6A33BA361D24}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8B9000-9193-4B8E-B7C6-27DEFEF68A5D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="793">
   <si>
     <t>name</t>
   </si>
@@ -2390,6 +2390,15 @@
   </si>
   <si>
     <t>True</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -2427,7 +2436,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2450,12 +2459,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2467,6 +2487,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -2773,10 +2796,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I130"/>
+  <dimension ref="A1:J130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+    <sheetView tabSelected="1" topLeftCell="E102" workbookViewId="0">
+      <selection activeCell="J130" sqref="J130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2791,7 +2814,7 @@
     <col min="9" max="9" width="63" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2819,8 +2842,11 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J1" s="7" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2848,8 +2874,11 @@
       <c r="I2" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -2877,8 +2906,11 @@
       <c r="I3" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -2906,8 +2938,11 @@
       <c r="I4" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J4" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -2935,8 +2970,11 @@
       <c r="I5" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="3" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>36</v>
       </c>
@@ -2964,8 +3002,11 @@
       <c r="I6" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J6" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>42</v>
       </c>
@@ -2993,8 +3034,11 @@
       <c r="I7" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J7" s="3" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -3022,8 +3066,11 @@
       <c r="I8" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J8" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>52</v>
       </c>
@@ -3051,8 +3098,11 @@
       <c r="I9" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>60</v>
       </c>
@@ -3080,8 +3130,11 @@
       <c r="I10" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J10" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -3109,8 +3162,11 @@
       <c r="I11" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J11" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>74</v>
       </c>
@@ -3138,8 +3194,11 @@
       <c r="I12" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>78</v>
       </c>
@@ -3167,8 +3226,11 @@
       <c r="I13" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J13" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>84</v>
       </c>
@@ -3196,8 +3258,11 @@
       <c r="I14" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J14" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>88</v>
       </c>
@@ -3225,8 +3290,11 @@
       <c r="I15" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J15" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>94</v>
       </c>
@@ -3254,8 +3322,11 @@
       <c r="I16" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J16" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>100</v>
       </c>
@@ -3283,8 +3354,11 @@
       <c r="I17" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J17" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>107</v>
       </c>
@@ -3312,8 +3386,11 @@
       <c r="I18" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J18" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>113</v>
       </c>
@@ -3341,8 +3418,11 @@
       <c r="I19" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J19" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>119</v>
       </c>
@@ -3370,8 +3450,11 @@
       <c r="I20" s="2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J20" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>125</v>
       </c>
@@ -3399,8 +3482,11 @@
       <c r="I21" s="2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J21" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>131</v>
       </c>
@@ -3428,8 +3514,11 @@
       <c r="I22" s="2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J22" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>137</v>
       </c>
@@ -3457,8 +3546,11 @@
       <c r="I23" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J23" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>145</v>
       </c>
@@ -3486,8 +3578,11 @@
       <c r="I24" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J24" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>149</v>
       </c>
@@ -3515,8 +3610,11 @@
       <c r="I25" s="2" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J25" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>153</v>
       </c>
@@ -3544,8 +3642,11 @@
       <c r="I26" s="2" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J26" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>157</v>
       </c>
@@ -3569,8 +3670,11 @@
       <c r="I27" s="2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J27" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>163</v>
       </c>
@@ -3598,8 +3702,11 @@
       <c r="I28" s="2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J28" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>167</v>
       </c>
@@ -3627,8 +3734,11 @@
       <c r="I29" s="2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J29" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>173</v>
       </c>
@@ -3656,8 +3766,11 @@
       <c r="I30" s="2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J30" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>179</v>
       </c>
@@ -3685,8 +3798,11 @@
       <c r="I31" s="2" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J31" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>185</v>
       </c>
@@ -3714,8 +3830,11 @@
       <c r="I32" s="2" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J32" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>189</v>
       </c>
@@ -3743,8 +3862,11 @@
       <c r="I33" s="2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J33" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>195</v>
       </c>
@@ -3772,8 +3894,11 @@
       <c r="I34" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J34" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>201</v>
       </c>
@@ -3801,8 +3926,11 @@
       <c r="I35" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J35" s="3" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>205</v>
       </c>
@@ -3830,8 +3958,11 @@
       <c r="I36" s="2" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J36" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>211</v>
       </c>
@@ -3859,8 +3990,11 @@
       <c r="I37" s="2" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J37" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>217</v>
       </c>
@@ -3888,8 +4022,11 @@
       <c r="I38" s="2" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J38" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>223</v>
       </c>
@@ -3917,8 +4054,11 @@
       <c r="I39" s="2" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J39" s="3" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>227</v>
       </c>
@@ -3946,8 +4086,11 @@
       <c r="I40" s="2" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J40" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>233</v>
       </c>
@@ -3975,8 +4118,11 @@
       <c r="I41" s="2" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J41" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>237</v>
       </c>
@@ -4004,8 +4150,11 @@
       <c r="I42" s="2" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J42" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>243</v>
       </c>
@@ -4033,8 +4182,11 @@
       <c r="I43" s="2" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J43" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>247</v>
       </c>
@@ -4058,8 +4210,11 @@
       <c r="I44" s="2" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J44" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>250</v>
       </c>
@@ -4087,8 +4242,11 @@
       <c r="I45" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J45" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>255</v>
       </c>
@@ -4116,8 +4274,11 @@
       <c r="I46" s="2" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J46" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>260</v>
       </c>
@@ -4141,8 +4302,11 @@
       <c r="I47" s="2" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J47" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>264</v>
       </c>
@@ -4170,8 +4334,11 @@
       <c r="I48" s="2" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J48" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>270</v>
       </c>
@@ -4199,8 +4366,11 @@
       <c r="I49" s="2" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J49" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>274</v>
       </c>
@@ -4228,8 +4398,11 @@
       <c r="I50" s="2" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J50" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>280</v>
       </c>
@@ -4257,8 +4430,11 @@
       <c r="I51" s="2" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J51" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>288</v>
       </c>
@@ -4286,8 +4462,11 @@
       <c r="I52" s="2" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J52" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>292</v>
       </c>
@@ -4315,8 +4494,11 @@
       <c r="I53" s="2" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J53" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>298</v>
       </c>
@@ -4344,8 +4526,11 @@
       <c r="I54" s="2" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J54" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>302</v>
       </c>
@@ -4373,8 +4558,11 @@
       <c r="I55" s="2" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J55" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>310</v>
       </c>
@@ -4402,8 +4590,11 @@
       <c r="I56" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J56" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>314</v>
       </c>
@@ -4431,8 +4622,11 @@
       <c r="I57" s="2" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J57" s="3" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>318</v>
       </c>
@@ -4460,8 +4654,11 @@
       <c r="I58" s="2" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J58" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>324</v>
       </c>
@@ -4489,8 +4686,11 @@
       <c r="I59" s="2" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J59" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>330</v>
       </c>
@@ -4518,8 +4718,11 @@
       <c r="I60" s="2" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J60" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>334</v>
       </c>
@@ -4547,8 +4750,11 @@
       <c r="I61" s="2" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J61" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>342</v>
       </c>
@@ -4576,8 +4782,11 @@
       <c r="I62" s="2" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J62" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>346</v>
       </c>
@@ -4605,8 +4814,11 @@
       <c r="I63" s="2" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J63" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>350</v>
       </c>
@@ -4634,8 +4846,11 @@
       <c r="I64" s="2" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J64" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>356</v>
       </c>
@@ -4663,8 +4878,11 @@
       <c r="I65" s="2" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J65" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>362</v>
       </c>
@@ -4692,8 +4910,11 @@
       <c r="I66" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J66" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>366</v>
       </c>
@@ -4721,8 +4942,11 @@
       <c r="I67" s="2" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J67" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>370</v>
       </c>
@@ -4750,8 +4974,11 @@
       <c r="I68" s="2" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J68" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>375</v>
       </c>
@@ -4772,8 +4999,11 @@
       <c r="I69" s="2" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J69" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>379</v>
       </c>
@@ -4801,8 +5031,11 @@
       <c r="I70" s="2" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J70" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>384</v>
       </c>
@@ -4830,8 +5063,11 @@
       <c r="I71" s="2" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J71" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>388</v>
       </c>
@@ -4859,8 +5095,11 @@
       <c r="I72" s="2" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J72" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>392</v>
       </c>
@@ -4888,8 +5127,11 @@
       <c r="I73" s="2" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J73" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>398</v>
       </c>
@@ -4917,8 +5159,11 @@
       <c r="I74" s="2" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J74" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>402</v>
       </c>
@@ -4946,8 +5191,11 @@
       <c r="I75" s="2" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J75" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>406</v>
       </c>
@@ -4975,8 +5223,11 @@
       <c r="I76" s="2" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J76" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>412</v>
       </c>
@@ -5004,8 +5255,11 @@
       <c r="I77" s="2" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J77" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>416</v>
       </c>
@@ -5033,8 +5287,11 @@
       <c r="I78" s="2" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J78" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>424</v>
       </c>
@@ -5062,8 +5319,11 @@
       <c r="I79" s="2" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J79" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>428</v>
       </c>
@@ -5091,8 +5351,11 @@
       <c r="I80" s="2" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J80" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>432</v>
       </c>
@@ -5120,8 +5383,11 @@
       <c r="I81" s="2" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J81" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>438</v>
       </c>
@@ -5149,8 +5415,11 @@
       <c r="I82" s="2" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J82" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>444</v>
       </c>
@@ -5178,8 +5447,11 @@
       <c r="I83" s="2" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J83" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>450</v>
       </c>
@@ -5200,8 +5472,11 @@
       <c r="I84" s="2" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J84" s="3" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>452</v>
       </c>
@@ -5229,8 +5504,11 @@
       <c r="I85" s="2" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J85" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>456</v>
       </c>
@@ -5258,8 +5536,11 @@
       <c r="I86" s="2" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J86" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>462</v>
       </c>
@@ -5287,8 +5568,11 @@
       <c r="I87" s="2" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J87" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>468</v>
       </c>
@@ -5316,8 +5600,11 @@
       <c r="I88" s="2" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J88" s="3" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>472</v>
       </c>
@@ -5345,8 +5632,11 @@
       <c r="I89" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J89" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>476</v>
       </c>
@@ -5374,8 +5664,11 @@
       <c r="I90" s="2" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J90" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>480</v>
       </c>
@@ -5403,8 +5696,11 @@
       <c r="I91" s="2" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J91" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>486</v>
       </c>
@@ -5432,8 +5728,11 @@
       <c r="I92" s="2" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J92" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>492</v>
       </c>
@@ -5461,8 +5760,11 @@
       <c r="I93" s="2" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J93" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>496</v>
       </c>
@@ -5490,8 +5792,11 @@
       <c r="I94" s="2" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J94" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>500</v>
       </c>
@@ -5519,8 +5824,11 @@
       <c r="I95" s="2" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J95" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>502</v>
       </c>
@@ -5548,8 +5856,11 @@
       <c r="I96" s="2" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J96" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>508</v>
       </c>
@@ -5577,8 +5888,11 @@
       <c r="I97" s="2" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J97" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>512</v>
       </c>
@@ -5606,8 +5920,11 @@
       <c r="I98" s="2" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J98" s="3" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>517</v>
       </c>
@@ -5635,8 +5952,11 @@
       <c r="I99" s="2" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J99" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>523</v>
       </c>
@@ -5657,8 +5977,11 @@
       <c r="I100" s="2" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J100" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>525</v>
       </c>
@@ -5686,8 +6009,11 @@
       <c r="I101" s="2" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J101" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>533</v>
       </c>
@@ -5712,8 +6038,11 @@
       <c r="I102" s="2" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J102" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>537</v>
       </c>
@@ -5741,8 +6070,11 @@
       <c r="I103" s="2" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J103" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>543</v>
       </c>
@@ -5770,8 +6102,11 @@
       <c r="I104" s="2" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J104" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>551</v>
       </c>
@@ -5799,8 +6134,11 @@
       <c r="I105" s="2" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J105" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>557</v>
       </c>
@@ -5828,8 +6166,11 @@
       <c r="I106" s="2" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J106" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>561</v>
       </c>
@@ -5857,8 +6198,11 @@
       <c r="I107" s="2" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J107" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>565</v>
       </c>
@@ -5886,8 +6230,11 @@
       <c r="I108" s="2" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J108" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>569</v>
       </c>
@@ -5915,8 +6262,11 @@
       <c r="I109" s="2" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J109" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>575</v>
       </c>
@@ -5940,8 +6290,11 @@
       <c r="I110" s="2" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J110" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>579</v>
       </c>
@@ -5969,8 +6322,11 @@
       <c r="I111" s="2" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J111" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>583</v>
       </c>
@@ -5998,8 +6354,11 @@
       <c r="I112" s="2" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J112" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>589</v>
       </c>
@@ -6027,8 +6386,11 @@
       <c r="I113" s="2" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J113" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>595</v>
       </c>
@@ -6056,8 +6418,11 @@
       <c r="I114" s="2" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J114" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>601</v>
       </c>
@@ -6085,8 +6450,11 @@
       <c r="I115" s="2" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J115" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>607</v>
       </c>
@@ -6114,8 +6482,11 @@
       <c r="I116" s="2" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="117" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J116" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>609</v>
       </c>
@@ -6143,8 +6514,11 @@
       <c r="I117" s="2" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J117" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>616</v>
       </c>
@@ -6172,8 +6546,11 @@
       <c r="I118" s="2" t="s">
         <v>621</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J118" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>622</v>
       </c>
@@ -6201,8 +6578,11 @@
       <c r="I119" s="2" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J119" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>626</v>
       </c>
@@ -6230,8 +6610,11 @@
       <c r="I120" s="2" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J120" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>632</v>
       </c>
@@ -6259,8 +6642,11 @@
       <c r="I121" s="2" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J121" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>638</v>
       </c>
@@ -6288,8 +6674,11 @@
       <c r="I122" s="2" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J122" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>644</v>
       </c>
@@ -6317,8 +6706,11 @@
       <c r="I123" s="2" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J123" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>648</v>
       </c>
@@ -6346,8 +6738,11 @@
       <c r="I124" s="2" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J124" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>652</v>
       </c>
@@ -6375,8 +6770,11 @@
       <c r="I125" s="2" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J125" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>658</v>
       </c>
@@ -6404,8 +6802,11 @@
       <c r="I126" s="2" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J126" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>666</v>
       </c>
@@ -6433,8 +6834,11 @@
       <c r="I127" s="2" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J127" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>670</v>
       </c>
@@ -6462,8 +6866,11 @@
       <c r="I128" s="2" t="s">
         <v>675</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J128" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>676</v>
       </c>
@@ -6491,8 +6898,11 @@
       <c r="I129" s="2" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J129" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>682</v>
       </c>
@@ -6519,6 +6929,9 @@
       </c>
       <c r="I130" s="2" t="s">
         <v>684</v>
+      </c>
+      <c r="J130" s="3" t="s">
+        <v>791</v>
       </c>
     </row>
   </sheetData>

</xml_diff>